<commit_message>
Added the lecture timetable script linking to the python script , edited the lecture timetable database , edited the upload students results to work properly with courses that doesn't have lab or section , edited the admit students results to show the students that needs 4~1 degrees to success
</commit_message>
<xml_diff>
--- a/app/scripts/lectures/Profs Time.xlsx
+++ b/app/scripts/lectures/Profs Time.xlsx
@@ -64,7 +64,7 @@
     <row r="1" spans="1:2" customHeight="0">
       <c r="A1" s="0" t="inlineStr">
         <is>
-          <t>Profs</t>
+          <t>profs</t>
         </is>
       </c>
       <c r="B1" s="0" t="inlineStr">
@@ -81,7 +81,19 @@
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>Sunday-2:00PM-3:30PM</t>
+          <t>Sunday-2:00PM:3:30PM,Sunday-12:30PM:2:00PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" spans="1:2" customHeight="0">
+      <c r="A3" s="0" t="inlineStr">
+        <is>
+          <t>Dr. Wendy Stokes</t>
+        </is>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>Sunday-9:00AM:10:30AM,Sunday-10:30AM:12:00PM,Sunday-12:30PM:2:00PM,Sunday-2:00PM:3:30PM,Sunday-3:30PM:5:00PM,Monday-9:00AM:10:30AM,Monday-10:30AM:12:00PM,Monday-12:30PM:2:00PM,Monday-2:00PM:3:30PM,Monday-3:30PM:5:00PM,Tuesday-9:00AM:10:30AM,Tuesday-10:30AM:12:00PM,Tuesday-12:30PM:2:00PM,Tuesday-2:00PM:3:30PM,Tuesday-3:30PM:5:00PM,Wednesday-9:00AM:10:30AM,Wednesday-10:30AM:12:00PM,Wednesday-12:30PM:2:00PM,Wednesday-2:00PM:3:30PM,Wednesday-3:30PM:5:00PM,Thursday-9:00AM:10:30AM,Thursday-10:30AM:12:00PM,Thursday-12:30PM:2:00PM,Thursday-2:00PM:3:30PM,Thursday-3:30PM:5:00PM,Friday-9:00AM:10:30AM,Friday-10:30AM:12:00PM,Friday-12:30PM:2:00PM,Friday-2:00PM:3:30PM,Friday-3:30PM:5:00PM,Saturday-9:00AM:10:30AM,Saturday-10:30AM:12:00PM,Saturday-12:30PM:2:00PM,Saturday-2:00PM:3:30PM,Saturday-3:30PM:5:00PM</t>
         </is>
       </c>
     </row>

</xml_diff>